<commit_message>
adding new keywords - assertPresent, assertEqual
</commit_message>
<xml_diff>
--- a/Raftaar/assets/testcase.xlsx
+++ b/Raftaar/assets/testcase.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="671">
   <si>
     <t>openBrowser</t>
   </si>
@@ -1924,9 +1924,6 @@
     <t>{normalize}</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>xpath=//button[@onclick='alertFunction()']</t>
   </si>
   <si>
@@ -2036,6 +2033,9 @@
   </si>
   <si>
     <t>no description</t>
+  </si>
+  <si>
+    <t>This is bit tricky. Webdriver don't have any in-build feature to validate this.</t>
   </si>
 </sst>
 </file>
@@ -2581,7 +2581,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2612,7 +2612,7 @@
         <v>134</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>400</v>
@@ -2621,34 +2621,34 @@
     </row>
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>62</v>
+        <v>159</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>87</v>
+        <v>160</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>400</v>
       </c>
-      <c r="D3" s="19"/>
+      <c r="D3" s="13"/>
     </row>
     <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>84</v>
+        <v>167</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>400</v>
       </c>
-      <c r="D4" s="19"/>
+      <c r="D4" s="13"/>
     </row>
     <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>400</v>
@@ -2657,10 +2657,10 @@
     </row>
     <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>2</v>
+        <v>84</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>88</v>
+        <v>179</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>400</v>
@@ -2669,10 +2669,10 @@
     </row>
     <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>400</v>
@@ -2681,10 +2681,10 @@
     </row>
     <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>68</v>
+        <v>2</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>194</v>
+        <v>88</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>400</v>
@@ -2693,10 +2693,10 @@
     </row>
     <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>400</v>
@@ -2705,10 +2705,10 @@
     </row>
     <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>98</v>
+        <v>194</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>400</v>
@@ -2717,10 +2717,10 @@
     </row>
     <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>400</v>
@@ -2729,10 +2729,10 @@
     </row>
     <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>400</v>
@@ -2741,10 +2741,10 @@
     </row>
     <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>316</v>
+        <v>80</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>317</v>
+        <v>90</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>400</v>
@@ -2753,10 +2753,10 @@
     </row>
     <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>1</v>
+        <v>65</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>400</v>
@@ -2765,34 +2765,34 @@
     </row>
     <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>200</v>
+        <v>316</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>201</v>
+        <v>317</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>400</v>
       </c>
-      <c r="D15" s="13"/>
+      <c r="D15" s="19"/>
     </row>
     <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>668</v>
+        <v>1</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>669</v>
+        <v>97</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>400</v>
       </c>
-      <c r="D16" s="13"/>
+      <c r="D16" s="19"/>
     </row>
     <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>400</v>
@@ -2801,34 +2801,34 @@
     </row>
     <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>4</v>
+        <v>667</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>9</v>
+        <v>668</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>400</v>
       </c>
-      <c r="D18" s="19"/>
+      <c r="D18" s="13"/>
     </row>
     <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>0</v>
+        <v>202</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C19" s="16" t="s">
         <v>400</v>
       </c>
-      <c r="D19" s="19"/>
+      <c r="D19" s="13"/>
     </row>
     <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>95</v>
+        <v>9</v>
       </c>
       <c r="C20" s="16" t="s">
         <v>400</v>
@@ -2837,58 +2837,58 @@
     </row>
     <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>207</v>
+        <v>0</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C21" s="16" t="s">
         <v>400</v>
       </c>
-      <c r="D21" s="13"/>
+      <c r="D21" s="19"/>
     </row>
     <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>83</v>
+        <v>23</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>623</v>
-      </c>
-      <c r="C22" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C22" s="16" t="s">
         <v>400</v>
       </c>
       <c r="D22" s="19"/>
     </row>
     <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>258</v>
+        <v>207</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>444</v>
+        <v>208</v>
       </c>
       <c r="C23" s="16" t="s">
         <v>400</v>
       </c>
-      <c r="D23" s="19"/>
+      <c r="D23" s="13"/>
     </row>
     <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="C24" s="16" t="s">
+        <v>623</v>
+      </c>
+      <c r="C24" s="17" t="s">
         <v>400</v>
       </c>
       <c r="D24" s="19"/>
     </row>
     <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>22</v>
+        <v>258</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>220</v>
+        <v>444</v>
       </c>
       <c r="C25" s="16" t="s">
         <v>400</v>
@@ -2897,10 +2897,10 @@
     </row>
     <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="C26" s="16" t="s">
         <v>400</v>
@@ -2909,10 +2909,10 @@
     </row>
     <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>92</v>
+        <v>220</v>
       </c>
       <c r="C27" s="16" t="s">
         <v>400</v>
@@ -2921,10 +2921,10 @@
     </row>
     <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>11</v>
+        <v>79</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="C28" s="16" t="s">
         <v>400</v>
@@ -2933,10 +2933,10 @@
     </row>
     <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>96</v>
+        <v>59</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>320</v>
+        <v>92</v>
       </c>
       <c r="C29" s="16" t="s">
         <v>400</v>
@@ -2945,10 +2945,10 @@
     </row>
     <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>93</v>
+        <v>11</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="C30" s="16" t="s">
         <v>400</v>
@@ -2957,10 +2957,10 @@
     </row>
     <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>94</v>
+        <v>320</v>
       </c>
       <c r="C31" s="16" t="s">
         <v>400</v>
@@ -2969,58 +2969,60 @@
     </row>
     <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
-        <v>250</v>
+        <v>93</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="C32" s="16" t="s">
         <v>400</v>
       </c>
       <c r="D32" s="19"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>130</v>
+        <v>85</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>630</v>
-      </c>
-      <c r="D33" s="20"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>400</v>
+      </c>
+      <c r="D33" s="19"/>
+    </row>
+    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
-        <v>137</v>
+        <v>250</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>630</v>
-      </c>
-      <c r="D34" s="20"/>
+        <v>251</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>400</v>
+      </c>
+      <c r="D34" s="19"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="C35" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="C35" s="14" t="s">
         <v>630</v>
       </c>
-      <c r="D35" s="20"/>
+      <c r="D35" s="13" t="s">
+        <v>635</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="C36" s="15" t="s">
         <v>630</v>
@@ -3029,10 +3031,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="C37" s="15" t="s">
         <v>630</v>
@@ -3041,10 +3043,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="C38" s="15" t="s">
         <v>630</v>
@@ -3053,10 +3055,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="C39" s="15" t="s">
         <v>630</v>
@@ -3065,10 +3067,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
-        <v>135</v>
+        <v>153</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>136</v>
+        <v>154</v>
       </c>
       <c r="C40" s="15" t="s">
         <v>630</v>
@@ -3077,10 +3079,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
-        <v>139</v>
+        <v>157</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>140</v>
+        <v>158</v>
       </c>
       <c r="C41" s="15" t="s">
         <v>630</v>
@@ -3089,10 +3091,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>162</v>
+        <v>133</v>
       </c>
       <c r="C42" s="15" t="s">
         <v>630</v>
@@ -3101,10 +3103,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
-        <v>175</v>
+        <v>135</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>176</v>
+        <v>136</v>
       </c>
       <c r="C43" s="15" t="s">
         <v>630</v>
@@ -3113,10 +3115,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
-        <v>173</v>
+        <v>139</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>174</v>
+        <v>140</v>
       </c>
       <c r="C44" s="15" t="s">
         <v>630</v>
@@ -3125,10 +3127,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
-        <v>266</v>
+        <v>161</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>267</v>
+        <v>162</v>
       </c>
       <c r="C45" s="15" t="s">
         <v>630</v>
@@ -3137,10 +3139,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
-        <v>302</v>
+        <v>175</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>303</v>
+        <v>176</v>
       </c>
       <c r="C46" s="15" t="s">
         <v>630</v>
@@ -3149,22 +3151,24 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
-        <v>337</v>
+        <v>163</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>338</v>
-      </c>
-      <c r="C47" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="C47" s="14" t="s">
         <v>630</v>
       </c>
-      <c r="D47" s="20"/>
+      <c r="D47" s="13" t="s">
+        <v>670</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
-        <v>272</v>
+        <v>173</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>273</v>
+        <v>174</v>
       </c>
       <c r="C48" s="15" t="s">
         <v>630</v>
@@ -3173,10 +3177,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
-        <v>325</v>
+        <v>266</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>326</v>
+        <v>267</v>
       </c>
       <c r="C49" s="15" t="s">
         <v>630</v>
@@ -3185,10 +3189,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
-        <v>182</v>
+        <v>302</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>183</v>
+        <v>303</v>
       </c>
       <c r="C50" s="15" t="s">
         <v>630</v>
@@ -3197,10 +3201,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
-        <v>351</v>
+        <v>337</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>352</v>
+        <v>338</v>
       </c>
       <c r="C51" s="15" t="s">
         <v>630</v>
@@ -3209,10 +3213,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="s">
-        <v>353</v>
+        <v>272</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>354</v>
+        <v>273</v>
       </c>
       <c r="C52" s="15" t="s">
         <v>630</v>
@@ -3221,10 +3225,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
-        <v>349</v>
+        <v>325</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>350</v>
+        <v>326</v>
       </c>
       <c r="C53" s="15" t="s">
         <v>630</v>
@@ -3233,10 +3237,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
-        <v>356</v>
+        <v>182</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>352</v>
+        <v>183</v>
       </c>
       <c r="C54" s="15" t="s">
         <v>630</v>
@@ -3245,10 +3249,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C55" s="15" t="s">
         <v>630</v>
@@ -3257,10 +3261,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="C56" s="15" t="s">
         <v>630</v>
@@ -3269,10 +3273,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
-        <v>341</v>
+        <v>349</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>342</v>
+        <v>350</v>
       </c>
       <c r="C57" s="15" t="s">
         <v>630</v>
@@ -3281,10 +3285,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
-        <v>278</v>
+        <v>356</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>279</v>
+        <v>352</v>
       </c>
       <c r="C58" s="15" t="s">
         <v>630</v>
@@ -3293,10 +3297,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="s">
-        <v>280</v>
+        <v>355</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>281</v>
+        <v>354</v>
       </c>
       <c r="C59" s="15" t="s">
         <v>630</v>
@@ -3305,10 +3309,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
-        <v>192</v>
+        <v>357</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>193</v>
+        <v>350</v>
       </c>
       <c r="C60" s="15" t="s">
         <v>630</v>
@@ -3317,10 +3321,10 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
-        <v>379</v>
+        <v>341</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>380</v>
+        <v>342</v>
       </c>
       <c r="C61" s="15" t="s">
         <v>630</v>
@@ -3329,10 +3333,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
-        <v>358</v>
+        <v>278</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>359</v>
+        <v>279</v>
       </c>
       <c r="C62" s="15" t="s">
         <v>630</v>
@@ -3341,10 +3345,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
-        <v>308</v>
+        <v>280</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>309</v>
+        <v>281</v>
       </c>
       <c r="C63" s="15" t="s">
         <v>630</v>
@@ -3353,10 +3357,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
-        <v>310</v>
+        <v>192</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>311</v>
+        <v>193</v>
       </c>
       <c r="C64" s="15" t="s">
         <v>630</v>
@@ -3365,10 +3369,10 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
-        <v>282</v>
+        <v>379</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>283</v>
+        <v>380</v>
       </c>
       <c r="C65" s="15" t="s">
         <v>630</v>
@@ -3377,10 +3381,10 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C66" s="15" t="s">
         <v>630</v>
@@ -3389,10 +3393,10 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
-        <v>284</v>
+        <v>308</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>285</v>
+        <v>309</v>
       </c>
       <c r="C67" s="15" t="s">
         <v>630</v>
@@ -3401,10 +3405,10 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="13" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="B68" s="13" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="C68" s="15" t="s">
         <v>630</v>
@@ -3413,10 +3417,10 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="13" t="s">
-        <v>362</v>
+        <v>282</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>363</v>
+        <v>283</v>
       </c>
       <c r="C69" s="15" t="s">
         <v>630</v>
@@ -3425,10 +3429,10 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="s">
-        <v>371</v>
+        <v>360</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>372</v>
+        <v>361</v>
       </c>
       <c r="C70" s="15" t="s">
         <v>630</v>
@@ -3437,10 +3441,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="13" t="s">
-        <v>373</v>
+        <v>284</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>374</v>
+        <v>285</v>
       </c>
       <c r="C71" s="15" t="s">
         <v>630</v>
@@ -3449,10 +3453,10 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="13" t="s">
-        <v>366</v>
+        <v>306</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>365</v>
+        <v>307</v>
       </c>
       <c r="C72" s="15" t="s">
         <v>630</v>
@@ -3461,10 +3465,10 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="13" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="C73" s="15" t="s">
         <v>630</v>
@@ -3473,10 +3477,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="13" t="s">
-        <v>255</v>
+        <v>371</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>256</v>
+        <v>372</v>
       </c>
       <c r="C74" s="15" t="s">
         <v>630</v>
@@ -3485,10 +3489,10 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="13" t="s">
-        <v>257</v>
+        <v>373</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>256</v>
+        <v>374</v>
       </c>
       <c r="C75" s="15" t="s">
         <v>630</v>
@@ -3497,10 +3501,10 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="13" t="s">
-        <v>209</v>
+        <v>366</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>210</v>
+        <v>365</v>
       </c>
       <c r="C76" s="15" t="s">
         <v>630</v>
@@ -3509,10 +3513,10 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="13" t="s">
-        <v>211</v>
+        <v>369</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>212</v>
+        <v>370</v>
       </c>
       <c r="C77" s="15" t="s">
         <v>630</v>
@@ -3521,10 +3525,10 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="13" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C78" s="15" t="s">
         <v>630</v>
@@ -3533,10 +3537,10 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="13" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B79" s="13" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C79" s="15" t="s">
         <v>630</v>
@@ -3545,10 +3549,10 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">
-        <v>300</v>
+        <v>209</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>301</v>
+        <v>210</v>
       </c>
       <c r="C80" s="15" t="s">
         <v>630</v>
@@ -3557,10 +3561,10 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="s">
-        <v>298</v>
+        <v>211</v>
       </c>
       <c r="B81" s="13" t="s">
-        <v>299</v>
+        <v>212</v>
       </c>
       <c r="C81" s="15" t="s">
         <v>630</v>
@@ -3569,10 +3573,10 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="s">
-        <v>304</v>
+        <v>254</v>
       </c>
       <c r="B82" s="13" t="s">
-        <v>305</v>
+        <v>253</v>
       </c>
       <c r="C82" s="15" t="s">
         <v>630</v>
@@ -3581,10 +3585,10 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
-        <v>214</v>
+        <v>260</v>
       </c>
       <c r="B83" s="13" t="s">
-        <v>215</v>
+        <v>259</v>
       </c>
       <c r="C83" s="15" t="s">
         <v>630</v>
@@ -3593,10 +3597,10 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="s">
-        <v>216</v>
+        <v>300</v>
       </c>
       <c r="B84" s="13" t="s">
-        <v>217</v>
+        <v>301</v>
       </c>
       <c r="C84" s="15" t="s">
         <v>630</v>
@@ -3605,10 +3609,10 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
-        <v>224</v>
+        <v>298</v>
       </c>
       <c r="B85" s="13" t="s">
-        <v>225</v>
+        <v>299</v>
       </c>
       <c r="C85" s="15" t="s">
         <v>630</v>
@@ -3617,10 +3621,10 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="s">
-        <v>226</v>
+        <v>304</v>
       </c>
       <c r="B86" s="13" t="s">
-        <v>227</v>
+        <v>305</v>
       </c>
       <c r="C86" s="15" t="s">
         <v>630</v>
@@ -3629,10 +3633,10 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
       <c r="B87" s="13" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="C87" s="15" t="s">
         <v>630</v>
@@ -3641,10 +3645,10 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
       <c r="B88" s="13" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
       <c r="C88" s="15" t="s">
         <v>630</v>
@@ -3653,10 +3657,10 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
-        <v>377</v>
+        <v>224</v>
       </c>
       <c r="B89" s="13" t="s">
-        <v>378</v>
+        <v>225</v>
       </c>
       <c r="C89" s="15" t="s">
         <v>630</v>
@@ -3665,10 +3669,10 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
-        <v>331</v>
+        <v>226</v>
       </c>
       <c r="B90" s="13" t="s">
-        <v>332</v>
+        <v>227</v>
       </c>
       <c r="C90" s="15" t="s">
         <v>630</v>
@@ -3677,10 +3681,10 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="B91" s="13" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="C91" s="15" t="s">
         <v>630</v>
@@ -3689,10 +3693,10 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="B92" s="13" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="C92" s="15" t="s">
         <v>630</v>
@@ -3701,10 +3705,10 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="13" t="s">
-        <v>323</v>
+        <v>377</v>
       </c>
       <c r="B93" s="13" t="s">
-        <v>324</v>
+        <v>378</v>
       </c>
       <c r="C93" s="15" t="s">
         <v>630</v>
@@ -3713,10 +3717,10 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="13" t="s">
-        <v>321</v>
+        <v>331</v>
       </c>
       <c r="B94" s="13" t="s">
-        <v>322</v>
+        <v>332</v>
       </c>
       <c r="C94" s="15" t="s">
         <v>630</v>
@@ -3725,10 +3729,10 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="13" t="s">
-        <v>263</v>
+        <v>239</v>
       </c>
       <c r="B95" s="13" t="s">
-        <v>264</v>
+        <v>240</v>
       </c>
       <c r="C95" s="15" t="s">
         <v>630</v>
@@ -3737,10 +3741,10 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="13" t="s">
-        <v>265</v>
+        <v>241</v>
       </c>
       <c r="B96" s="13" t="s">
-        <v>264</v>
+        <v>242</v>
       </c>
       <c r="C96" s="15" t="s">
         <v>630</v>
@@ -3749,10 +3753,10 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="13" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="B97" s="13" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="C97" s="15" t="s">
         <v>630</v>
@@ -3761,10 +3765,10 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="13" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="B98" s="13" t="s">
-        <v>336</v>
+        <v>322</v>
       </c>
       <c r="C98" s="15" t="s">
         <v>630</v>
@@ -3773,10 +3777,10 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="13" t="s">
-        <v>244</v>
+        <v>263</v>
       </c>
       <c r="B99" s="13" t="s">
-        <v>245</v>
+        <v>264</v>
       </c>
       <c r="C99" s="15" t="s">
         <v>630</v>
@@ -3785,10 +3789,10 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="13" t="s">
-        <v>246</v>
+        <v>265</v>
       </c>
       <c r="B100" s="13" t="s">
-        <v>247</v>
+        <v>264</v>
       </c>
       <c r="C100" s="15" t="s">
         <v>630</v>
@@ -3797,10 +3801,10 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="13" t="s">
-        <v>375</v>
+        <v>333</v>
       </c>
       <c r="B101" s="13" t="s">
-        <v>376</v>
+        <v>334</v>
       </c>
       <c r="C101" s="15" t="s">
         <v>630</v>
@@ -3809,58 +3813,58 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="13" t="s">
-        <v>177</v>
+        <v>335</v>
       </c>
       <c r="B102" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="C102" s="14" t="s">
-        <v>633</v>
-      </c>
-      <c r="D102" s="13" t="s">
-        <v>636</v>
-      </c>
+        <v>336</v>
+      </c>
+      <c r="C102" s="15" t="s">
+        <v>630</v>
+      </c>
+      <c r="D102" s="20"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="13" t="s">
-        <v>268</v>
+        <v>244</v>
       </c>
       <c r="B103" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="C103" s="14" t="s">
-        <v>619</v>
-      </c>
-      <c r="D103" s="13"/>
+        <v>245</v>
+      </c>
+      <c r="C103" s="15" t="s">
+        <v>630</v>
+      </c>
+      <c r="D103" s="20"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="13" t="s">
-        <v>631</v>
-      </c>
-      <c r="B104" s="13"/>
-      <c r="C104" s="14" t="s">
-        <v>619</v>
-      </c>
-      <c r="D104" s="13"/>
+        <v>246</v>
+      </c>
+      <c r="B104" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="C104" s="15" t="s">
+        <v>630</v>
+      </c>
+      <c r="D104" s="20"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="13" t="s">
-        <v>147</v>
+        <v>375</v>
       </c>
       <c r="B105" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="C105" s="14" t="s">
-        <v>619</v>
-      </c>
-      <c r="D105" s="13"/>
+        <v>376</v>
+      </c>
+      <c r="C105" s="15" t="s">
+        <v>630</v>
+      </c>
+      <c r="D105" s="20"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="13" t="s">
-        <v>145</v>
+        <v>268</v>
       </c>
       <c r="B106" s="13" t="s">
-        <v>146</v>
+        <v>269</v>
       </c>
       <c r="C106" s="14" t="s">
         <v>619</v>
@@ -3869,11 +3873,9 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="B107" s="13" t="s">
-        <v>150</v>
-      </c>
+        <v>631</v>
+      </c>
+      <c r="B107" s="13"/>
       <c r="C107" s="14" t="s">
         <v>619</v>
       </c>
@@ -3881,10 +3883,10 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="13" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B108" s="13" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C108" s="14" t="s">
         <v>619</v>
@@ -3893,10 +3895,10 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="13" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="B109" s="13" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="C109" s="14" t="s">
         <v>619</v>
@@ -3905,10 +3907,10 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="13" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="B110" s="13" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="C110" s="14" t="s">
         <v>619</v>
@@ -3917,10 +3919,10 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="13" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="B111" s="13" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="C111" s="14" t="s">
         <v>619</v>
@@ -3929,10 +3931,10 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="13" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B112" s="13" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C112" s="14" t="s">
         <v>619</v>
@@ -3941,10 +3943,10 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B113" s="13" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C113" s="14" t="s">
         <v>619</v>
@@ -4412,7 +4414,7 @@
         <v>622</v>
       </c>
       <c r="B152" s="13" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C152" s="14" t="s">
         <v>619</v>
@@ -4424,7 +4426,7 @@
         <v>621</v>
       </c>
       <c r="B153" s="13" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C153" s="14" t="s">
         <v>619</v>
@@ -8376,7 +8378,7 @@
         <v>1</v>
       </c>
       <c r="G193" s="11" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="H193" s="6"/>
       <c r="I193" s="6"/>
@@ -24779,7 +24781,7 @@
       </c>
       <c r="D195" s="6"/>
       <c r="E195" s="6" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="F195" s="6" t="s">
         <v>2</v>
@@ -24815,13 +24817,13 @@
     </row>
     <row r="198" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A198" s="6" t="s">
+        <v>636</v>
+      </c>
+      <c r="B198" s="5" t="s">
         <v>637</v>
       </c>
-      <c r="B198" s="5" t="s">
+      <c r="C198" s="6" t="s">
         <v>638</v>
-      </c>
-      <c r="C198" s="6" t="s">
-        <v>639</v>
       </c>
       <c r="E198" s="12">
         <v>5</v>
@@ -24835,7 +24837,7 @@
     </row>
     <row r="199" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A199" s="6" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B199" s="5" t="s">
         <v>548</v>
@@ -24844,36 +24846,36 @@
         <v>549</v>
       </c>
       <c r="F199" s="6" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="200" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="C200" s="5" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="F200" s="5" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="201" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="C201" s="5" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="F201" s="5" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="202" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="C202" s="5" t="s">
+        <v>646</v>
+      </c>
+      <c r="F202" s="5" t="s">
         <v>647</v>
-      </c>
-      <c r="F202" s="5" t="s">
-        <v>648</v>
       </c>
     </row>
     <row r="203" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A203" s="6" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B203" s="5" t="s">
         <v>549</v>
@@ -24890,10 +24892,10 @@
     </row>
     <row r="204" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A204" s="5" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B204" s="5" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C204" s="6" t="s">
         <v>394</v>
@@ -24909,13 +24911,13 @@
     </row>
     <row r="205" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A205" s="5" t="s">
+        <v>644</v>
+      </c>
+      <c r="B205" s="5" t="s">
+        <v>640</v>
+      </c>
+      <c r="C205" s="1" t="s">
         <v>645</v>
-      </c>
-      <c r="B205" s="5" t="s">
-        <v>641</v>
-      </c>
-      <c r="C205" s="1" t="s">
-        <v>646</v>
       </c>
       <c r="D205" s="6"/>
       <c r="E205" s="6"/>
@@ -24926,10 +24928,10 @@
     </row>
     <row r="206" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A206" s="5" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B206" s="5" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C206" s="6" t="s">
         <v>9</v>
@@ -24943,13 +24945,13 @@
     </row>
     <row r="207" spans="1:16384" ht="15" x14ac:dyDescent="0.2">
       <c r="A207" s="6" t="s">
+        <v>648</v>
+      </c>
+      <c r="B207" s="6" t="s">
         <v>649</v>
       </c>
-      <c r="B207" s="6" t="s">
+      <c r="C207" s="6" t="s">
         <v>650</v>
-      </c>
-      <c r="C207" s="6" t="s">
-        <v>651</v>
       </c>
       <c r="D207" s="6"/>
       <c r="E207" s="6"/>
@@ -24957,7 +24959,7 @@
         <v>0</v>
       </c>
       <c r="G207" s="11" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="H207" s="6"/>
       <c r="I207" s="6"/>
@@ -24970,13 +24972,13 @@
       </c>
       <c r="D208" s="6"/>
       <c r="E208" s="6" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="F208" s="6" t="s">
         <v>11</v>
       </c>
       <c r="G208" s="11" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="H208" s="6"/>
       <c r="I208" s="6"/>
@@ -24989,7 +24991,7 @@
       </c>
       <c r="D209" s="6"/>
       <c r="E209" s="6" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="F209" s="6" t="s">
         <v>93</v>
@@ -25004,11 +25006,11 @@
       <c r="A210" s="6"/>
       <c r="B210" s="6"/>
       <c r="C210" s="6" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="D210" s="6"/>
       <c r="E210" s="6" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="F210" s="6" t="s">
         <v>2</v>
@@ -25021,11 +25023,11 @@
       <c r="A211" s="6"/>
       <c r="B211" s="6"/>
       <c r="C211" s="6" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D211" s="6"/>
       <c r="E211" s="6" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="F211" s="6" t="s">
         <v>85</v>
@@ -25040,11 +25042,11 @@
       <c r="A212" s="6"/>
       <c r="B212" s="6"/>
       <c r="C212" s="6" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="D212" s="6"/>
       <c r="E212" s="6" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="F212" s="6" t="s">
         <v>2</v>
@@ -25057,11 +25059,11 @@
       <c r="A213" s="6"/>
       <c r="B213" s="6"/>
       <c r="C213" s="6" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D213" s="6"/>
       <c r="E213" s="6" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="F213" s="6" t="s">
         <v>85</v>
@@ -25076,17 +25078,17 @@
       <c r="A214" s="6"/>
       <c r="B214" s="6"/>
       <c r="C214" s="6" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="D214" s="6"/>
       <c r="E214" s="6" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="F214" s="6" t="s">
         <v>68</v>
       </c>
       <c r="G214" s="6" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="H214" s="6"/>
       <c r="I214" s="6"/>
@@ -25095,17 +25097,17 @@
       <c r="A215" s="6"/>
       <c r="B215" s="6"/>
       <c r="C215" s="6" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="D215" s="6"/>
       <c r="E215" s="6" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="F215" s="6" t="s">
         <v>62</v>
       </c>
       <c r="G215" s="6" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="H215" s="6"/>
       <c r="I215" s="6"/>

</xml_diff>